<commit_message>
[Document, Modified]: ManageProject Usecase Specification
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Document/Diagram/UseCase/ManageProject/ManageProject Specification.xlsx
+++ b/ToDoApp-Doc/Document/Diagram/UseCase/ManageProject/ManageProject Specification.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="53">
   <si>
     <t xml:space="preserve">Use-case number:</t>
   </si>
@@ -176,27 +176,21 @@
     <t xml:space="preserve">1. Nhấp chọn “More actions” trên trực tiếp project.</t>
   </si>
   <si>
-    <t xml:space="preserve">2. Hiển thị danh mục các tùy chọn.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3. Nhấp chọn “Update”.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4. Hiển thị giao diện cập nhật project.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5. Nhập tên project mới.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">6. Kiểm tra tên project </t>
+    <t xml:space="preserve">2. Hiển thị giao diện cập nhật project.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Nhập tên project mới.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">4. Kiểm tra tên project </t>
     </r>
     <r>
       <rPr>
@@ -207,19 +201,29 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">E1.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">7. Nhấp chọn “Save” </t>
+      <t xml:space="preserve">E1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">5. Nhấp chọn “Save” </t>
     </r>
     <r>
       <rPr>
@@ -242,6 +246,9 @@
       </rPr>
       <t xml:space="preserve">.</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">6. Cập nhật project.</t>
   </si>
   <si>
     <r>
@@ -702,8 +709,8 @@
   </sheetPr>
   <dimension ref="B2:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -809,73 +816,59 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="5"/>
-      <c r="C14" s="4" t="s">
+    <row r="14" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="5"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D19" s="4"/>
-    </row>
-    <row r="20" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="4"/>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -886,13 +879,13 @@
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="B7:B15"/>
+    <mergeCell ref="B7:B13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
   </mergeCells>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -934,7 +927,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" s="4"/>
     </row>
@@ -943,7 +936,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="4"/>
     </row>
@@ -961,7 +954,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="4"/>
     </row>
@@ -979,7 +972,7 @@
     <row r="8" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="5"/>
       <c r="C8" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="4"/>
     </row>
@@ -987,13 +980,13 @@
       <c r="B9" s="5"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="5"/>
       <c r="C10" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="4"/>
     </row>
@@ -1001,7 +994,7 @@
       <c r="B11" s="5"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1009,7 +1002,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" s="3"/>
     </row>
@@ -1036,7 +1029,7 @@
         <v>24</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15" s="4"/>
     </row>
@@ -1045,7 +1038,7 @@
         <v>26</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D16" s="4"/>
     </row>
@@ -1054,7 +1047,7 @@
         <v>28</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D17" s="4"/>
     </row>

</xml_diff>